<commit_message>
Added FD0810004 to database
</commit_message>
<xml_diff>
--- a/To Add v2/Clock&Timing - Oscillators  - Fixed - Logic_Out.xlsx
+++ b/To Add v2/Clock&Timing - Oscillators  - Fixed - Logic_Out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\To Add v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Danakil_KiCad_DB\To Add v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3E92F1-D6DF-4AD9-B9C9-9122BF42ACCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0CA580-1510-473B-9A42-659DFC667884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Totals</t>
   </si>
@@ -156,6 +156,30 @@
   </si>
   <si>
     <t>0Dan_Clock&amp;Timing - Oscillators  - Fixed - Logic_Out:ECS-2520MVLC-081.92</t>
+  </si>
+  <si>
+    <t>FD0810004-ND</t>
+  </si>
+  <si>
+    <t>FD0810004</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>2.97-3.63v</t>
+  </si>
+  <si>
+    <t>5x3mm</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/FD_3-3V.pdf</t>
+  </si>
+  <si>
+    <t>0Dan_Clock&amp;Timing - Oscillators  - Fixed - Logic_Out:FD0810004</t>
+  </si>
+  <si>
+    <t>Osc_Logic_Out:FD0810_DIO</t>
   </si>
 </sst>
 </file>
@@ -489,100 +513,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Z7"/>
+  <dimension ref="B1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="12" max="12" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" customWidth="1"/>
+    <col min="12" max="12" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
         <f>COUNTA(C7:C9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:R2" si="0">COUNTA(D7:D9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <f>COUNTA(E7:E9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2" si="1">COUNTA(F7:F9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f>COUNTA(G7:G9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2" si="2">COUNTA(H7:H9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f>COUNTA(I7:I9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2" si="3">COUNTA(J7:J9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" t="s">
         <v>1</v>
@@ -592,16 +616,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
       <c r="Y3" t="s">
         <v>2</v>
       </c>
       <c r="Z3">
         <f>MAX(C2:R2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -658,10 +682,10 @@
       </c>
       <c r="Z4">
         <f>SUM(W7:W9999)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="Y5" t="s">
         <v>5</v>
       </c>
@@ -670,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -729,7 +753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="C7" t="str">
         <f>_xlfn.CONCAT(E7,F7," ",H7," ",G7," ",J7," ",I7," ",R7)</f>
         <v>8.192MHz±25PPM 1.6-3.6v CMOS XO 2.5x2.0mm  </v>
@@ -798,6 +822,70 @@
       <c r="Z7">
         <f>SUM(C4:R4)</f>
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(E8,F8," ",H8," ",G8," ",J8," ",I8," ",R8)</f>
+        <v>8.192MHz±25PPM 2.97-3.63v CMOS XO 5x3mm  </v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xlfn.CONCAT(E8," ",J8)</f>
+        <v>8.192MHz XO</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8">
+        <f>COUNTBLANK(C8:R8)</f>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f>100*COUNTA(C8:R8)/$Z$7</f>
+        <v>100</v>
+      </c>
+      <c r="W8">
+        <f>IF(V8=100,1,0)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>